<commit_message>
Revised lineage template to allow selecting the process type
Signed-off-by: Christopher Grote <cmgrote@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/atlan-documentation-template.xlsx
+++ b/atlan-documentation-template.xlsx
@@ -155,13 +155,19 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="K1">
+    <comment authorId="0" ref="F2">
+      <text>
+        <t xml:space="preserve">Also required, this indicates the type of orchestration process. This influences the icon you will see for the lineage process, and the combination of this and the orchestrator will uniquely identify the connection in which the lineage process is created.
+	-Chris Grote</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="L1">
       <text>
         <t xml:space="preserve">These fields are all optional. Any data that is provided for these fields will be attached to the lineage process itself, not to the source or target assets.
 	-Chris Grote</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2">
+    <comment authorId="0" ref="G2">
       <text>
         <t xml:space="preserve">This ID uniquely identifies all the inputs used and outputs produced by a single granular job within the orchestrator
 	-Chris Grote</t>
@@ -179,7 +185,7 @@
 	-Chris Grote</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2">
+    <comment authorId="0" ref="I2">
       <text>
         <t xml:space="preserve">This column is always required, to indicate the type of the target asset
 	-Chris Grote</t>
@@ -191,7 +197,7 @@
 	-Chris Grote</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2">
+    <comment authorId="0" ref="H2">
       <text>
         <t xml:space="preserve">This can be either:
 - The full qualifiedName of the target asset. In this case, the "Connector (t)" and "Connection (t)" columns are ignored.
@@ -212,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="186">
   <si>
     <t>Connection</t>
   </si>
@@ -616,6 +622,36 @@
     <t>Object containing miscallaneous information tracked in January 2023</t>
   </si>
   <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>Connection for raw (unresolved) lineage against underlying S3 objects</t>
+  </si>
+  <si>
+    <t>dev-atlan-sources</t>
+  </si>
+  <si>
+    <t>s3://dev-atlan-sources</t>
+  </si>
+  <si>
+    <t>INSTACART_ORDERS_MASTER.csv</t>
+  </si>
+  <si>
+    <t>s3://dev-atlan-sources/sample-data/instacart/INSTACART_ORDERS_MASTER/</t>
+  </si>
+  <si>
+    <t>file/csv</t>
+  </si>
+  <si>
+    <t>output_dataset.parquet</t>
+  </si>
+  <si>
+    <t>s3://dev-atlan-sources/somewhere/else/output_dataset.parquet</t>
+  </si>
+  <si>
+    <t>file/parquet</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
@@ -643,6 +679,9 @@
     <t>Orchestrator</t>
   </si>
   <si>
+    <t>Process Type</t>
+  </si>
+  <si>
     <t>Process ID</t>
   </si>
   <si>
@@ -670,6 +709,9 @@
     <t>DataGrip</t>
   </si>
   <si>
+    <t>api</t>
+  </si>
+  <si>
     <t>ide_1</t>
   </si>
   <si>
@@ -697,6 +739,9 @@
     <t>MWAA</t>
   </si>
   <si>
+    <t>airflow</t>
+  </si>
+  <si>
     <t>mwaa_dag_1</t>
   </si>
   <si>
@@ -716,6 +761,23 @@
   </si>
   <si>
     <t>https://airflow.apache.org/</t>
+  </si>
+  <si>
+    <t>mwaa_dag_001</t>
+  </si>
+  <si>
+    <t>df = aws.read_parquet(“arn::s3:::/dev-atlan-sources/sample-data/instacart/INSTACART_ORDERS_MASTER.csv”)
+df = df[‘geoography_mapped_value’] = df.geography_type.apply(lambda y: 1 if y == "City" else 0)
+aws.write_parquet(df, “arn::s3:::/dev-atlan-sources/somewhere/else/output_dataset.parquet”)</t>
+  </si>
+  <si>
+    <t>Transformation of raw S3 objects, without going through any query layer</t>
+  </si>
+  <si>
+    <t>mwaa_dag_002</t>
+  </si>
+  <si>
+    <t>default/athena/1674058491/AwsDataCatalog/instacart/instacart_orders_master</t>
   </si>
 </sst>
 </file>
@@ -3471,8 +3533,12 @@
       <c r="S12" s="14"/>
     </row>
     <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -3481,7 +3547,9 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -3492,11 +3560,19 @@
       <c r="S13" s="14"/>
     </row>
     <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>137</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -3513,16 +3589,32 @@
       <c r="S14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="D15" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>139</v>
+      </c>
       <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="10">
+        <v>1.05372834E8</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>140</v>
+      </c>
       <c r="K15" s="13"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
@@ -3534,16 +3626,32 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>142</v>
+      </c>
       <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="I16" s="10">
+        <v>7382347.0</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="K16" s="13"/>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
@@ -4512,45 +4620,47 @@
     <col customWidth="1" min="2" max="2" width="12.63"/>
     <col customWidth="1" min="3" max="3" width="15.88"/>
     <col customWidth="1" min="4" max="4" width="30.88"/>
-    <col customWidth="1" min="5" max="6" width="11.5"/>
-    <col customWidth="1" min="7" max="7" width="24.88"/>
-    <col customWidth="1" min="8" max="8" width="15.25"/>
-    <col customWidth="1" min="9" max="9" width="11.5"/>
-    <col customWidth="1" min="10" max="10" width="12.25"/>
-    <col customWidth="1" min="11" max="11" width="20.38"/>
-    <col customWidth="1" min="12" max="12" width="54.38"/>
-    <col customWidth="1" min="13" max="13" width="40.88"/>
-    <col customWidth="1" min="14" max="14" width="11.13"/>
-    <col customWidth="1" min="15" max="15" width="16.63"/>
-    <col customWidth="1" min="16" max="16" width="13.13"/>
-    <col customWidth="1" min="17" max="17" width="17.0"/>
-    <col customWidth="1" min="18" max="18" width="20.63"/>
-    <col customWidth="1" min="19" max="19" width="11.25"/>
-    <col customWidth="1" min="20" max="20" width="12.63"/>
-    <col customWidth="1" min="21" max="21" width="12.75"/>
+    <col customWidth="1" min="5" max="5" width="11.5"/>
+    <col customWidth="1" min="6" max="6" width="11.75"/>
+    <col customWidth="1" min="7" max="7" width="11.5"/>
+    <col customWidth="1" min="8" max="8" width="24.88"/>
+    <col customWidth="1" min="9" max="9" width="15.25"/>
+    <col customWidth="1" min="10" max="10" width="11.5"/>
+    <col customWidth="1" min="11" max="11" width="12.25"/>
+    <col customWidth="1" min="12" max="12" width="20.38"/>
+    <col customWidth="1" min="13" max="13" width="54.38"/>
+    <col customWidth="1" min="14" max="14" width="40.88"/>
+    <col customWidth="1" min="15" max="15" width="11.13"/>
+    <col customWidth="1" min="16" max="16" width="16.63"/>
+    <col customWidth="1" min="17" max="17" width="13.13"/>
+    <col customWidth="1" min="18" max="18" width="17.0"/>
+    <col customWidth="1" min="19" max="19" width="20.63"/>
+    <col customWidth="1" min="20" max="20" width="11.25"/>
+    <col customWidth="1" min="21" max="21" width="12.63"/>
+    <col customWidth="1" min="22" max="22" width="12.75"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="19" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="20"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
-      <c r="K1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="L1" s="6"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -4560,69 +4670,73 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>144</v>
+        <v>153</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>154</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>146</v>
+        <v>155</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>148</v>
+        <v>157</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4637,43 +4751,46 @@
         <v>72</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>153</v>
+        <v>163</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="H3" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="J3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="K3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="N3" s="13"/>
+      <c r="L3" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>168</v>
+      </c>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="14"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="14"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
@@ -4686,39 +4803,42 @@
         <v>72</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>157</v>
+        <v>163</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="H4" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="M4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="25" t="s">
+        <v>167</v>
+      </c>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="14"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="14"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
@@ -4731,39 +4851,42 @@
         <v>72</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>157</v>
+        <v>163</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>170</v>
       </c>
       <c r="H5" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="J5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="K5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="M5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="26" t="s">
+        <v>167</v>
+      </c>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="14"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="14"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
@@ -4773,42 +4896,45 @@
         <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>112</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>153</v>
+        <v>173</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>174</v>
       </c>
       <c r="H6" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="J6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="K6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="M6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="25" t="s">
+        <v>175</v>
+      </c>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="14"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="14"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
@@ -4818,78 +4944,128 @@
         <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>157</v>
+        <v>173</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>179</v>
       </c>
       <c r="H7" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="J7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="K7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="M7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="25" t="s">
+        <v>180</v>
+      </c>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="14"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="14"/>
     </row>
     <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="A8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="14"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="14"/>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
+      <c r="A9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>72</v>
+      </c>
       <c r="J9" s="24"/>
-      <c r="K9" s="13"/>
+      <c r="K9" s="24"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -4897,9 +5073,10 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="14"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="14"/>
     </row>
     <row r="10">
       <c r="A10" s="7"/>
@@ -4908,11 +5085,11 @@
       <c r="D10" s="8"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
+      <c r="I10" s="23"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="24"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -4920,9 +5097,10 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="14"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="7"/>
@@ -4931,11 +5109,11 @@
       <c r="D11" s="8"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="24"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -4943,9 +5121,10 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="14"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="14"/>
     </row>
     <row r="12">
       <c r="A12" s="7"/>
@@ -4954,11 +5133,11 @@
       <c r="D12" s="8"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="24"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="24"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -4966,9 +5145,10 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="14"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="14"/>
     </row>
     <row r="13">
       <c r="A13" s="7"/>
@@ -4977,11 +5157,11 @@
       <c r="D13" s="8"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="24"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="24"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -4989,9 +5169,10 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="14"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="14"/>
     </row>
     <row r="14">
       <c r="A14" s="7"/>
@@ -5000,11 +5181,11 @@
       <c r="D14" s="8"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
+      <c r="I14" s="23"/>
       <c r="J14" s="24"/>
-      <c r="K14" s="13"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
@@ -5012,9 +5193,10 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="14"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="14"/>
     </row>
     <row r="15">
       <c r="A15" s="7"/>
@@ -5023,11 +5205,11 @@
       <c r="D15" s="8"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
+      <c r="I15" s="23"/>
       <c r="J15" s="24"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -5035,9 +5217,10 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="14"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="14"/>
     </row>
     <row r="16">
       <c r="A16" s="7"/>
@@ -5046,11 +5229,11 @@
       <c r="D16" s="8"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
+      <c r="I16" s="23"/>
       <c r="J16" s="24"/>
-      <c r="K16" s="13"/>
+      <c r="K16" s="24"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
@@ -5058,9 +5241,10 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="14"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="14"/>
     </row>
     <row r="17">
       <c r="A17" s="7"/>
@@ -5069,11 +5253,11 @@
       <c r="D17" s="8"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
+      <c r="I17" s="23"/>
       <c r="J17" s="24"/>
-      <c r="K17" s="13"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
@@ -5081,9 +5265,10 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="14"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="14"/>
     </row>
     <row r="18">
       <c r="A18" s="7"/>
@@ -5092,11 +5277,11 @@
       <c r="D18" s="8"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
+      <c r="I18" s="23"/>
       <c r="J18" s="24"/>
-      <c r="K18" s="13"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
@@ -5104,9 +5289,10 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="14"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="14"/>
     </row>
     <row r="19">
       <c r="A19" s="7"/>
@@ -5115,11 +5301,11 @@
       <c r="D19" s="8"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="13"/>
+      <c r="K19" s="24"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
@@ -5127,9 +5313,10 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="14"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="14"/>
     </row>
     <row r="20">
       <c r="A20" s="7"/>
@@ -5138,11 +5325,11 @@
       <c r="D20" s="8"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="24"/>
-      <c r="K20" s="13"/>
+      <c r="K20" s="24"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
@@ -5150,9 +5337,10 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="14"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="14"/>
     </row>
     <row r="21">
       <c r="A21" s="7"/>
@@ -5161,11 +5349,11 @@
       <c r="D21" s="8"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
+      <c r="I21" s="23"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="13"/>
+      <c r="K21" s="24"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
@@ -5173,9 +5361,10 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="14"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="14"/>
     </row>
     <row r="22">
       <c r="A22" s="7"/>
@@ -5184,11 +5373,11 @@
       <c r="D22" s="8"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="24"/>
-      <c r="K22" s="13"/>
+      <c r="K22" s="24"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
@@ -5196,9 +5385,10 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="14"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="14"/>
     </row>
     <row r="23">
       <c r="A23" s="7"/>
@@ -5207,11 +5397,11 @@
       <c r="D23" s="8"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="24"/>
-      <c r="K23" s="13"/>
+      <c r="K23" s="24"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
@@ -5219,9 +5409,10 @@
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="14"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="14"/>
     </row>
     <row r="24">
       <c r="A24" s="7"/>
@@ -5230,11 +5421,11 @@
       <c r="D24" s="8"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="23"/>
-      <c r="I24" s="24"/>
+      <c r="I24" s="23"/>
       <c r="J24" s="24"/>
-      <c r="K24" s="13"/>
+      <c r="K24" s="24"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>
@@ -5242,9 +5433,10 @@
       <c r="P24" s="13"/>
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="14"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="14"/>
     </row>
     <row r="25">
       <c r="A25" s="7"/>
@@ -5253,11 +5445,11 @@
       <c r="D25" s="8"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
+      <c r="I25" s="23"/>
       <c r="J25" s="24"/>
-      <c r="K25" s="13"/>
+      <c r="K25" s="24"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
@@ -5265,9 +5457,10 @@
       <c r="P25" s="13"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="14"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="14"/>
     </row>
     <row r="26">
       <c r="A26" s="7"/>
@@ -5276,11 +5469,11 @@
       <c r="D26" s="8"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
+      <c r="I26" s="23"/>
       <c r="J26" s="24"/>
-      <c r="K26" s="13"/>
+      <c r="K26" s="24"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
@@ -5288,9 +5481,10 @@
       <c r="P26" s="13"/>
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="14"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="14"/>
     </row>
     <row r="27">
       <c r="A27" s="7"/>
@@ -5299,11 +5493,11 @@
       <c r="D27" s="8"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="22"/>
       <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
+      <c r="I27" s="23"/>
       <c r="J27" s="24"/>
-      <c r="K27" s="13"/>
+      <c r="K27" s="24"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
@@ -5311,9 +5505,10 @@
       <c r="P27" s="13"/>
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="14"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="14"/>
     </row>
     <row r="28">
       <c r="A28" s="7"/>
@@ -5322,11 +5517,11 @@
       <c r="D28" s="8"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
-      <c r="G28" s="23"/>
+      <c r="G28" s="22"/>
       <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
+      <c r="I28" s="23"/>
       <c r="J28" s="24"/>
-      <c r="K28" s="13"/>
+      <c r="K28" s="24"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
@@ -5334,9 +5529,10 @@
       <c r="P28" s="13"/>
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="14"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="14"/>
     </row>
     <row r="29">
       <c r="A29" s="7"/>
@@ -5345,11 +5541,11 @@
       <c r="D29" s="8"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="23"/>
-      <c r="I29" s="24"/>
+      <c r="I29" s="23"/>
       <c r="J29" s="24"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="24"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
@@ -5357,9 +5553,10 @@
       <c r="P29" s="13"/>
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="13"/>
-      <c r="U29" s="14"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
     </row>
     <row r="30">
       <c r="A30" s="7"/>
@@ -5368,11 +5565,11 @@
       <c r="D30" s="8"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="G30" s="22"/>
       <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
+      <c r="I30" s="23"/>
       <c r="J30" s="24"/>
-      <c r="K30" s="13"/>
+      <c r="K30" s="24"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
@@ -5380,9 +5577,10 @@
       <c r="P30" s="13"/>
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="14"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="14"/>
     </row>
     <row r="31">
       <c r="A31" s="7"/>
@@ -5391,11 +5589,11 @@
       <c r="D31" s="8"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
+      <c r="I31" s="23"/>
       <c r="J31" s="24"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="24"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
@@ -5403,9 +5601,10 @@
       <c r="P31" s="13"/>
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="14"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="14"/>
     </row>
     <row r="32">
       <c r="A32" s="7"/>
@@ -5414,11 +5613,11 @@
       <c r="D32" s="8"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
-      <c r="G32" s="23"/>
+      <c r="G32" s="22"/>
       <c r="H32" s="23"/>
-      <c r="I32" s="24"/>
+      <c r="I32" s="23"/>
       <c r="J32" s="24"/>
-      <c r="K32" s="13"/>
+      <c r="K32" s="24"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
@@ -5426,9 +5625,10 @@
       <c r="P32" s="13"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="13"/>
-      <c r="U32" s="14"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="14"/>
     </row>
     <row r="33">
       <c r="A33" s="7"/>
@@ -5437,11 +5637,11 @@
       <c r="D33" s="8"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
-      <c r="G33" s="23"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
+      <c r="I33" s="23"/>
       <c r="J33" s="24"/>
-      <c r="K33" s="13"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
@@ -5449,9 +5649,10 @@
       <c r="P33" s="13"/>
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="13"/>
-      <c r="U33" s="14"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="14"/>
     </row>
     <row r="34">
       <c r="A34" s="7"/>
@@ -5460,11 +5661,11 @@
       <c r="D34" s="8"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
-      <c r="G34" s="23"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
+      <c r="I34" s="23"/>
       <c r="J34" s="24"/>
-      <c r="K34" s="13"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
@@ -5472,9 +5673,10 @@
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="13"/>
-      <c r="U34" s="14"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="14"/>
     </row>
     <row r="35">
       <c r="A35" s="7"/>
@@ -5483,11 +5685,11 @@
       <c r="D35" s="8"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
-      <c r="G35" s="23"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="23"/>
-      <c r="I35" s="24"/>
+      <c r="I35" s="23"/>
       <c r="J35" s="24"/>
-      <c r="K35" s="13"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
@@ -5495,9 +5697,10 @@
       <c r="P35" s="13"/>
       <c r="Q35" s="13"/>
       <c r="R35" s="13"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="14"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="14"/>
     </row>
     <row r="36">
       <c r="A36" s="7"/>
@@ -5506,11 +5709,11 @@
       <c r="D36" s="8"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
-      <c r="G36" s="23"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="23"/>
-      <c r="I36" s="24"/>
+      <c r="I36" s="23"/>
       <c r="J36" s="24"/>
-      <c r="K36" s="13"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
@@ -5518,9 +5721,10 @@
       <c r="P36" s="13"/>
       <c r="Q36" s="13"/>
       <c r="R36" s="13"/>
-      <c r="S36" s="14"/>
-      <c r="T36" s="13"/>
-      <c r="U36" s="14"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="14"/>
     </row>
     <row r="37">
       <c r="A37" s="7"/>
@@ -5529,11 +5733,11 @@
       <c r="D37" s="8"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
-      <c r="G37" s="23"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="23"/>
-      <c r="I37" s="24"/>
+      <c r="I37" s="23"/>
       <c r="J37" s="24"/>
-      <c r="K37" s="13"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
@@ -5541,9 +5745,10 @@
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
       <c r="R37" s="13"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="13"/>
-      <c r="U37" s="14"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="14"/>
     </row>
     <row r="38">
       <c r="A38" s="7"/>
@@ -5552,11 +5757,11 @@
       <c r="D38" s="8"/>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
-      <c r="G38" s="23"/>
+      <c r="G38" s="22"/>
       <c r="H38" s="23"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="23"/>
       <c r="J38" s="24"/>
-      <c r="K38" s="13"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
@@ -5564,9 +5769,10 @@
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="13"/>
-      <c r="U38" s="14"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="14"/>
     </row>
     <row r="39">
       <c r="A39" s="7"/>
@@ -5575,11 +5781,11 @@
       <c r="D39" s="8"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
-      <c r="G39" s="23"/>
+      <c r="G39" s="22"/>
       <c r="H39" s="23"/>
-      <c r="I39" s="24"/>
+      <c r="I39" s="23"/>
       <c r="J39" s="24"/>
-      <c r="K39" s="13"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
       <c r="N39" s="13"/>
@@ -5587,9 +5793,10 @@
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
-      <c r="S39" s="14"/>
-      <c r="T39" s="13"/>
-      <c r="U39" s="14"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="14"/>
     </row>
     <row r="40">
       <c r="A40" s="7"/>
@@ -5598,11 +5805,11 @@
       <c r="D40" s="8"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
-      <c r="G40" s="23"/>
+      <c r="G40" s="22"/>
       <c r="H40" s="23"/>
-      <c r="I40" s="24"/>
+      <c r="I40" s="23"/>
       <c r="J40" s="24"/>
-      <c r="K40" s="13"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
       <c r="N40" s="13"/>
@@ -5610,9 +5817,10 @@
       <c r="P40" s="13"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="13"/>
-      <c r="U40" s="14"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="14"/>
     </row>
     <row r="41">
       <c r="A41" s="7"/>
@@ -5621,11 +5829,11 @@
       <c r="D41" s="8"/>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
-      <c r="G41" s="23"/>
+      <c r="G41" s="22"/>
       <c r="H41" s="23"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="23"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="13"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
       <c r="N41" s="13"/>
@@ -5633,9 +5841,10 @@
       <c r="P41" s="13"/>
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
-      <c r="S41" s="14"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="14"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="14"/>
     </row>
     <row r="42">
       <c r="A42" s="7"/>
@@ -5644,11 +5853,11 @@
       <c r="D42" s="8"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
+      <c r="G42" s="22"/>
       <c r="H42" s="23"/>
-      <c r="I42" s="24"/>
+      <c r="I42" s="23"/>
       <c r="J42" s="24"/>
-      <c r="K42" s="13"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
       <c r="N42" s="13"/>
@@ -5656,9 +5865,10 @@
       <c r="P42" s="13"/>
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="13"/>
-      <c r="U42" s="14"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="14"/>
     </row>
     <row r="43">
       <c r="A43" s="7"/>
@@ -5667,11 +5877,11 @@
       <c r="D43" s="8"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="G43" s="22"/>
       <c r="H43" s="23"/>
-      <c r="I43" s="24"/>
+      <c r="I43" s="23"/>
       <c r="J43" s="24"/>
-      <c r="K43" s="13"/>
+      <c r="K43" s="24"/>
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
       <c r="N43" s="13"/>
@@ -5679,9 +5889,10 @@
       <c r="P43" s="13"/>
       <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="13"/>
-      <c r="U43" s="14"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="14"/>
     </row>
     <row r="44">
       <c r="A44" s="7"/>
@@ -5690,11 +5901,11 @@
       <c r="D44" s="8"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
-      <c r="G44" s="23"/>
+      <c r="G44" s="22"/>
       <c r="H44" s="23"/>
-      <c r="I44" s="24"/>
+      <c r="I44" s="23"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="13"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
       <c r="N44" s="13"/>
@@ -5702,9 +5913,10 @@
       <c r="P44" s="13"/>
       <c r="Q44" s="13"/>
       <c r="R44" s="13"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="13"/>
-      <c r="U44" s="14"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="14"/>
     </row>
     <row r="45">
       <c r="A45" s="7"/>
@@ -5713,11 +5925,11 @@
       <c r="D45" s="8"/>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
-      <c r="G45" s="23"/>
+      <c r="G45" s="22"/>
       <c r="H45" s="23"/>
-      <c r="I45" s="24"/>
+      <c r="I45" s="23"/>
       <c r="J45" s="24"/>
-      <c r="K45" s="13"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
@@ -5725,9 +5937,10 @@
       <c r="P45" s="13"/>
       <c r="Q45" s="13"/>
       <c r="R45" s="13"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="13"/>
-      <c r="U45" s="14"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="14"/>
     </row>
     <row r="46">
       <c r="A46" s="7"/>
@@ -5736,11 +5949,11 @@
       <c r="D46" s="8"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
-      <c r="G46" s="23"/>
+      <c r="G46" s="22"/>
       <c r="H46" s="23"/>
-      <c r="I46" s="24"/>
+      <c r="I46" s="23"/>
       <c r="J46" s="24"/>
-      <c r="K46" s="13"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="13"/>
       <c r="M46" s="13"/>
       <c r="N46" s="13"/>
@@ -5748,9 +5961,10 @@
       <c r="P46" s="13"/>
       <c r="Q46" s="13"/>
       <c r="R46" s="13"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="14"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="14"/>
     </row>
     <row r="47">
       <c r="A47" s="7"/>
@@ -5759,11 +5973,11 @@
       <c r="D47" s="8"/>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
-      <c r="G47" s="23"/>
+      <c r="G47" s="22"/>
       <c r="H47" s="23"/>
-      <c r="I47" s="24"/>
+      <c r="I47" s="23"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="13"/>
+      <c r="K47" s="24"/>
       <c r="L47" s="13"/>
       <c r="M47" s="13"/>
       <c r="N47" s="13"/>
@@ -5771,9 +5985,10 @@
       <c r="P47" s="13"/>
       <c r="Q47" s="13"/>
       <c r="R47" s="13"/>
-      <c r="S47" s="14"/>
-      <c r="T47" s="13"/>
-      <c r="U47" s="14"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="14"/>
     </row>
     <row r="48">
       <c r="A48" s="7"/>
@@ -5782,11 +5997,11 @@
       <c r="D48" s="8"/>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
-      <c r="G48" s="23"/>
+      <c r="G48" s="22"/>
       <c r="H48" s="23"/>
-      <c r="I48" s="24"/>
+      <c r="I48" s="23"/>
       <c r="J48" s="24"/>
-      <c r="K48" s="13"/>
+      <c r="K48" s="24"/>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
       <c r="N48" s="13"/>
@@ -5794,9 +6009,10 @@
       <c r="P48" s="13"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
-      <c r="S48" s="14"/>
-      <c r="T48" s="13"/>
-      <c r="U48" s="14"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="14"/>
     </row>
     <row r="49">
       <c r="A49" s="7"/>
@@ -5805,11 +6021,11 @@
       <c r="D49" s="8"/>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
-      <c r="G49" s="23"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="23"/>
-      <c r="I49" s="24"/>
+      <c r="I49" s="23"/>
       <c r="J49" s="24"/>
-      <c r="K49" s="13"/>
+      <c r="K49" s="24"/>
       <c r="L49" s="13"/>
       <c r="M49" s="13"/>
       <c r="N49" s="13"/>
@@ -5817,9 +6033,10 @@
       <c r="P49" s="13"/>
       <c r="Q49" s="13"/>
       <c r="R49" s="13"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="13"/>
-      <c r="U49" s="14"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="14"/>
     </row>
     <row r="50">
       <c r="A50" s="7"/>
@@ -5828,11 +6045,11 @@
       <c r="D50" s="8"/>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
-      <c r="G50" s="23"/>
+      <c r="G50" s="22"/>
       <c r="H50" s="23"/>
-      <c r="I50" s="24"/>
+      <c r="I50" s="23"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="13"/>
+      <c r="K50" s="24"/>
       <c r="L50" s="13"/>
       <c r="M50" s="13"/>
       <c r="N50" s="13"/>
@@ -5840,9 +6057,10 @@
       <c r="P50" s="13"/>
       <c r="Q50" s="13"/>
       <c r="R50" s="13"/>
-      <c r="S50" s="14"/>
-      <c r="T50" s="13"/>
-      <c r="U50" s="14"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="14"/>
     </row>
     <row r="51">
       <c r="A51" s="7"/>
@@ -5851,11 +6069,11 @@
       <c r="D51" s="8"/>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
-      <c r="G51" s="23"/>
+      <c r="G51" s="22"/>
       <c r="H51" s="23"/>
-      <c r="I51" s="24"/>
+      <c r="I51" s="23"/>
       <c r="J51" s="24"/>
-      <c r="K51" s="13"/>
+      <c r="K51" s="24"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
@@ -5863,9 +6081,10 @@
       <c r="P51" s="13"/>
       <c r="Q51" s="13"/>
       <c r="R51" s="13"/>
-      <c r="S51" s="14"/>
-      <c r="T51" s="13"/>
-      <c r="U51" s="14"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="14"/>
     </row>
     <row r="52">
       <c r="A52" s="7"/>
@@ -5874,11 +6093,11 @@
       <c r="D52" s="8"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
-      <c r="G52" s="23"/>
+      <c r="G52" s="22"/>
       <c r="H52" s="23"/>
-      <c r="I52" s="24"/>
+      <c r="I52" s="23"/>
       <c r="J52" s="24"/>
-      <c r="K52" s="13"/>
+      <c r="K52" s="24"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
@@ -5886,9 +6105,10 @@
       <c r="P52" s="13"/>
       <c r="Q52" s="13"/>
       <c r="R52" s="13"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="13"/>
-      <c r="U52" s="14"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="14"/>
     </row>
     <row r="53">
       <c r="A53" s="7"/>
@@ -5897,11 +6117,11 @@
       <c r="D53" s="8"/>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
-      <c r="G53" s="23"/>
+      <c r="G53" s="22"/>
       <c r="H53" s="23"/>
-      <c r="I53" s="24"/>
+      <c r="I53" s="23"/>
       <c r="J53" s="24"/>
-      <c r="K53" s="13"/>
+      <c r="K53" s="24"/>
       <c r="L53" s="13"/>
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
@@ -5909,9 +6129,10 @@
       <c r="P53" s="13"/>
       <c r="Q53" s="13"/>
       <c r="R53" s="13"/>
-      <c r="S53" s="14"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="14"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="14"/>
     </row>
     <row r="54">
       <c r="A54" s="7"/>
@@ -5920,11 +6141,11 @@
       <c r="D54" s="8"/>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
-      <c r="G54" s="23"/>
+      <c r="G54" s="22"/>
       <c r="H54" s="23"/>
-      <c r="I54" s="24"/>
+      <c r="I54" s="23"/>
       <c r="J54" s="24"/>
-      <c r="K54" s="13"/>
+      <c r="K54" s="24"/>
       <c r="L54" s="13"/>
       <c r="M54" s="13"/>
       <c r="N54" s="13"/>
@@ -5932,9 +6153,10 @@
       <c r="P54" s="13"/>
       <c r="Q54" s="13"/>
       <c r="R54" s="13"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="13"/>
-      <c r="U54" s="14"/>
+      <c r="S54" s="13"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="13"/>
+      <c r="V54" s="14"/>
     </row>
     <row r="55">
       <c r="A55" s="7"/>
@@ -5943,11 +6165,11 @@
       <c r="D55" s="8"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
-      <c r="G55" s="23"/>
+      <c r="G55" s="22"/>
       <c r="H55" s="23"/>
-      <c r="I55" s="24"/>
+      <c r="I55" s="23"/>
       <c r="J55" s="24"/>
-      <c r="K55" s="13"/>
+      <c r="K55" s="24"/>
       <c r="L55" s="13"/>
       <c r="M55" s="13"/>
       <c r="N55" s="13"/>
@@ -5955,9 +6177,10 @@
       <c r="P55" s="13"/>
       <c r="Q55" s="13"/>
       <c r="R55" s="13"/>
-      <c r="S55" s="14"/>
-      <c r="T55" s="13"/>
-      <c r="U55" s="14"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="14"/>
     </row>
     <row r="56">
       <c r="A56" s="7"/>
@@ -5966,11 +6189,11 @@
       <c r="D56" s="8"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
-      <c r="G56" s="23"/>
+      <c r="G56" s="22"/>
       <c r="H56" s="23"/>
-      <c r="I56" s="24"/>
+      <c r="I56" s="23"/>
       <c r="J56" s="24"/>
-      <c r="K56" s="13"/>
+      <c r="K56" s="24"/>
       <c r="L56" s="13"/>
       <c r="M56" s="13"/>
       <c r="N56" s="13"/>
@@ -5978,9 +6201,10 @@
       <c r="P56" s="13"/>
       <c r="Q56" s="13"/>
       <c r="R56" s="13"/>
-      <c r="S56" s="14"/>
-      <c r="T56" s="13"/>
-      <c r="U56" s="14"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="14"/>
+      <c r="U56" s="13"/>
+      <c r="V56" s="14"/>
     </row>
     <row r="57">
       <c r="A57" s="7"/>
@@ -5989,11 +6213,11 @@
       <c r="D57" s="8"/>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
-      <c r="G57" s="23"/>
+      <c r="G57" s="22"/>
       <c r="H57" s="23"/>
-      <c r="I57" s="24"/>
+      <c r="I57" s="23"/>
       <c r="J57" s="24"/>
-      <c r="K57" s="13"/>
+      <c r="K57" s="24"/>
       <c r="L57" s="13"/>
       <c r="M57" s="13"/>
       <c r="N57" s="13"/>
@@ -6001,9 +6225,10 @@
       <c r="P57" s="13"/>
       <c r="Q57" s="13"/>
       <c r="R57" s="13"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="13"/>
-      <c r="U57" s="14"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="14"/>
     </row>
     <row r="58">
       <c r="A58" s="7"/>
@@ -6012,11 +6237,11 @@
       <c r="D58" s="8"/>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
-      <c r="G58" s="23"/>
+      <c r="G58" s="22"/>
       <c r="H58" s="23"/>
-      <c r="I58" s="24"/>
+      <c r="I58" s="23"/>
       <c r="J58" s="24"/>
-      <c r="K58" s="13"/>
+      <c r="K58" s="24"/>
       <c r="L58" s="13"/>
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
@@ -6024,9 +6249,10 @@
       <c r="P58" s="13"/>
       <c r="Q58" s="13"/>
       <c r="R58" s="13"/>
-      <c r="S58" s="14"/>
-      <c r="T58" s="13"/>
-      <c r="U58" s="14"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="14"/>
+      <c r="U58" s="13"/>
+      <c r="V58" s="14"/>
     </row>
     <row r="59">
       <c r="A59" s="7"/>
@@ -6035,11 +6261,11 @@
       <c r="D59" s="8"/>
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
-      <c r="G59" s="23"/>
+      <c r="G59" s="22"/>
       <c r="H59" s="23"/>
-      <c r="I59" s="24"/>
+      <c r="I59" s="23"/>
       <c r="J59" s="24"/>
-      <c r="K59" s="13"/>
+      <c r="K59" s="24"/>
       <c r="L59" s="13"/>
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
@@ -6047,9 +6273,10 @@
       <c r="P59" s="13"/>
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
-      <c r="S59" s="14"/>
-      <c r="T59" s="13"/>
-      <c r="U59" s="14"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="13"/>
+      <c r="V59" s="14"/>
     </row>
     <row r="60">
       <c r="A60" s="7"/>
@@ -6058,11 +6285,11 @@
       <c r="D60" s="8"/>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
-      <c r="G60" s="23"/>
+      <c r="G60" s="22"/>
       <c r="H60" s="23"/>
-      <c r="I60" s="24"/>
+      <c r="I60" s="23"/>
       <c r="J60" s="24"/>
-      <c r="K60" s="13"/>
+      <c r="K60" s="24"/>
       <c r="L60" s="13"/>
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
@@ -6070,33 +6297,38 @@
       <c r="P60" s="13"/>
       <c r="Q60" s="13"/>
       <c r="R60" s="13"/>
-      <c r="S60" s="14"/>
-      <c r="T60" s="13"/>
-      <c r="U60" s="14"/>
+      <c r="S60" s="13"/>
+      <c r="T60" s="14"/>
+      <c r="U60" s="13"/>
+      <c r="V60" s="14"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:A60 I3:I60">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A3:A60 J3:J60">
       <formula1>"adls,api,athena,bigquery,databricks,datastudio,dynamodb,gcs,glue,hive,looker,metabase,mode,mssql,mysql,netsuite,oracle,postgres,powerbi,preset,presto,redshift,s3,salesforce,sap-hana,snowflake,trino,vertica,tableau"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3:N60">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F60">
+      <formula1>"airflow,api,dataflow,openlineage"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O3:O60">
       <formula1>"VERIFIED,DRAFT,DEPRECATED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C3:C7 H3:H7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C3:C60 I3:I60">
       <formula1>"ADLSObject,APIPath,DataStudioAsset,GCSObject,LookerDashboard,LookerExplore,LookerLook,LookerModel,LookerQuery,LookerTile,LookerView,MaterialisedView,MetabaseDashboard,MetabaseQuestion,ModeChart,ModeCollection,ModeQuery,ModeReport,PowerBIDashboard,PowerBID"&amp;"ataflow,PowerBIDataset,PowerBIDatasource,PowerBIMeasure,PowerBIPage,PowerBIReport,PowerBITable,PowerBITile,PresetChart,PresetDashboard,PresetDataset,S3Object,SalesforceDashboard,SalesforceObject,SalesforceReport,Table,TableauDashboard,TableauDatasource,Ta"&amp;"bleauFlow,TableauMetric,TableauWorksheet,View"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P3:P60">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q3:Q60">
       <formula1>"information,warning,issue"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="L3"/>
-    <hyperlink r:id="rId3" ref="L4"/>
-    <hyperlink r:id="rId4" ref="L5"/>
-    <hyperlink r:id="rId5" ref="L6"/>
-    <hyperlink r:id="rId6" ref="L7"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M4"/>
+    <hyperlink r:id="rId4" ref="M5"/>
+    <hyperlink r:id="rId5" ref="M6"/>
+    <hyperlink r:id="rId6" ref="M7"/>
+    <hyperlink r:id="rId7" ref="M8"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <drawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>